<commit_message>
Update prediction data and metrics in JSON; modify generation timestamp and adjust ARIMA parameters for improved accuracy.
</commit_message>
<xml_diff>
--- a/predicciones_produccion.xlsx
+++ b/predicciones_produccion.xlsx
@@ -471,19 +471,19 @@
         <v>45931</v>
       </c>
       <c r="B2" t="n">
-        <v>9088615.515252177</v>
+        <v>8850211.927541619</v>
       </c>
       <c r="C2" t="n">
-        <v>9088615.515252177</v>
+        <v>8850211.927541619</v>
       </c>
       <c r="D2" t="n">
-        <v>9088615.515252177</v>
+        <v>8850211.927541619</v>
       </c>
       <c r="E2" t="n">
-        <v>9088615.515252177</v>
+        <v>8850211.927541619</v>
       </c>
       <c r="F2" t="n">
-        <v>9088615.515252177</v>
+        <v>8850211.927541619</v>
       </c>
     </row>
     <row r="3">
@@ -491,19 +491,19 @@
         <v>45962</v>
       </c>
       <c r="B3" t="n">
-        <v>9088615.515252177</v>
+        <v>8850211.927541619</v>
       </c>
       <c r="C3" t="n">
-        <v>9088615.515252177</v>
+        <v>8850211.927541619</v>
       </c>
       <c r="D3" t="n">
-        <v>9088615.515252177</v>
+        <v>8850211.927541619</v>
       </c>
       <c r="E3" t="n">
-        <v>9088615.515252177</v>
+        <v>8850211.927541619</v>
       </c>
       <c r="F3" t="n">
-        <v>9088615.515252177</v>
+        <v>8850211.927541619</v>
       </c>
     </row>
     <row r="4">
@@ -511,19 +511,19 @@
         <v>45992</v>
       </c>
       <c r="B4" t="n">
-        <v>9088615.515252177</v>
+        <v>8850211.927541619</v>
       </c>
       <c r="C4" t="n">
-        <v>9088615.515252177</v>
+        <v>8850211.927541619</v>
       </c>
       <c r="D4" t="n">
-        <v>9088615.515252177</v>
+        <v>8850211.927541619</v>
       </c>
       <c r="E4" t="n">
-        <v>9088615.515252177</v>
+        <v>8850211.927541619</v>
       </c>
       <c r="F4" t="n">
-        <v>9088615.515252177</v>
+        <v>8850211.927541619</v>
       </c>
     </row>
     <row r="5">
@@ -531,19 +531,19 @@
         <v>46023</v>
       </c>
       <c r="B5" t="n">
-        <v>9088615.515252177</v>
+        <v>8850211.927541619</v>
       </c>
       <c r="C5" t="n">
-        <v>9088615.515252177</v>
+        <v>8850211.927541619</v>
       </c>
       <c r="D5" t="n">
-        <v>9088615.515252177</v>
+        <v>8850211.927541619</v>
       </c>
       <c r="E5" t="n">
-        <v>9088615.515252177</v>
+        <v>8850211.927541619</v>
       </c>
       <c r="F5" t="n">
-        <v>9088615.515252177</v>
+        <v>8850211.927541619</v>
       </c>
     </row>
     <row r="6">
@@ -551,19 +551,19 @@
         <v>46054</v>
       </c>
       <c r="B6" t="n">
-        <v>9088615.515252177</v>
+        <v>8850211.927541619</v>
       </c>
       <c r="C6" t="n">
-        <v>9088615.515252177</v>
+        <v>8850211.927541619</v>
       </c>
       <c r="D6" t="n">
-        <v>9088615.515252177</v>
+        <v>8850211.927541619</v>
       </c>
       <c r="E6" t="n">
-        <v>9088615.515252177</v>
+        <v>8850211.927541619</v>
       </c>
       <c r="F6" t="n">
-        <v>9088615.515252177</v>
+        <v>8850211.927541619</v>
       </c>
     </row>
     <row r="7">
@@ -571,19 +571,19 @@
         <v>46082</v>
       </c>
       <c r="B7" t="n">
-        <v>9088615.515252177</v>
+        <v>8850211.927541619</v>
       </c>
       <c r="C7" t="n">
-        <v>9088615.515252177</v>
+        <v>8850211.927541619</v>
       </c>
       <c r="D7" t="n">
-        <v>9088615.515252177</v>
+        <v>8850211.927541619</v>
       </c>
       <c r="E7" t="n">
-        <v>9088615.515252177</v>
+        <v>8850211.927541619</v>
       </c>
       <c r="F7" t="n">
-        <v>9088615.515252177</v>
+        <v>8850211.927541619</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implementación del modelo de series temporales con ARIMA y Prophet
- Se creó la clase ModeloSeriesTiempo para manejar la preparación, entrenamiento y evaluación de modelos de series temporales.
- Se implementaron métodos para preparar datos, analizar series, encontrar el mejor modelo ARIMA, y entrenar modelos ARIMA y Prophet.
- Se añadió funcionalidad para realizar predicciones futuras y visualizar resultados con intervalos de confianza.
- Se generó un reporte ejecutivo con resúmenes históricos y recomendaciones basadas en las predicciones.
- Se creó un script de ejemplo para demostrar el uso del modelo con datos simulados.

Adicionalmente, se desarrolló un script de ejemplo para cargar datos desde un archivo Excel y realizar predicciones utilizando el modelo híbrido.
</commit_message>
<xml_diff>
--- a/predicciones_produccion.xlsx
+++ b/predicciones_produccion.xlsx
@@ -471,19 +471,19 @@
         <v>45931</v>
       </c>
       <c r="B2" t="n">
-        <v>8850211.927541619</v>
+        <v>9241454.34912899</v>
       </c>
       <c r="C2" t="n">
-        <v>8850211.927541619</v>
+        <v>9241454.34912899</v>
       </c>
       <c r="D2" t="n">
-        <v>8850211.927541619</v>
+        <v>9241454.34912899</v>
       </c>
       <c r="E2" t="n">
-        <v>8850211.927541619</v>
+        <v>9241454.34912899</v>
       </c>
       <c r="F2" t="n">
-        <v>8850211.927541619</v>
+        <v>9241454.34912899</v>
       </c>
     </row>
     <row r="3">
@@ -491,19 +491,19 @@
         <v>45962</v>
       </c>
       <c r="B3" t="n">
-        <v>8850211.927541619</v>
+        <v>9241454.34912899</v>
       </c>
       <c r="C3" t="n">
-        <v>8850211.927541619</v>
+        <v>9241454.34912899</v>
       </c>
       <c r="D3" t="n">
-        <v>8850211.927541619</v>
+        <v>9241454.34912899</v>
       </c>
       <c r="E3" t="n">
-        <v>8850211.927541619</v>
+        <v>9241454.34912899</v>
       </c>
       <c r="F3" t="n">
-        <v>8850211.927541619</v>
+        <v>9241454.34912899</v>
       </c>
     </row>
     <row r="4">
@@ -511,19 +511,19 @@
         <v>45992</v>
       </c>
       <c r="B4" t="n">
-        <v>8850211.927541619</v>
+        <v>9241454.34912899</v>
       </c>
       <c r="C4" t="n">
-        <v>8850211.927541619</v>
+        <v>9241454.34912899</v>
       </c>
       <c r="D4" t="n">
-        <v>8850211.927541619</v>
+        <v>9241454.34912899</v>
       </c>
       <c r="E4" t="n">
-        <v>8850211.927541619</v>
+        <v>9241454.34912899</v>
       </c>
       <c r="F4" t="n">
-        <v>8850211.927541619</v>
+        <v>9241454.34912899</v>
       </c>
     </row>
     <row r="5">
@@ -531,19 +531,19 @@
         <v>46023</v>
       </c>
       <c r="B5" t="n">
-        <v>8850211.927541619</v>
+        <v>9241454.34912899</v>
       </c>
       <c r="C5" t="n">
-        <v>8850211.927541619</v>
+        <v>9241454.34912899</v>
       </c>
       <c r="D5" t="n">
-        <v>8850211.927541619</v>
+        <v>9241454.34912899</v>
       </c>
       <c r="E5" t="n">
-        <v>8850211.927541619</v>
+        <v>9241454.34912899</v>
       </c>
       <c r="F5" t="n">
-        <v>8850211.927541619</v>
+        <v>9241454.34912899</v>
       </c>
     </row>
     <row r="6">
@@ -551,19 +551,19 @@
         <v>46054</v>
       </c>
       <c r="B6" t="n">
-        <v>8850211.927541619</v>
+        <v>9241454.34912899</v>
       </c>
       <c r="C6" t="n">
-        <v>8850211.927541619</v>
+        <v>9241454.34912899</v>
       </c>
       <c r="D6" t="n">
-        <v>8850211.927541619</v>
+        <v>9241454.34912899</v>
       </c>
       <c r="E6" t="n">
-        <v>8850211.927541619</v>
+        <v>9241454.34912899</v>
       </c>
       <c r="F6" t="n">
-        <v>8850211.927541619</v>
+        <v>9241454.34912899</v>
       </c>
     </row>
     <row r="7">
@@ -571,19 +571,19 @@
         <v>46082</v>
       </c>
       <c r="B7" t="n">
-        <v>8850211.927541619</v>
+        <v>9241454.34912899</v>
       </c>
       <c r="C7" t="n">
-        <v>8850211.927541619</v>
+        <v>9241454.34912899</v>
       </c>
       <c r="D7" t="n">
-        <v>8850211.927541619</v>
+        <v>9241454.34912899</v>
       </c>
       <c r="E7" t="n">
-        <v>8850211.927541619</v>
+        <v>9241454.34912899</v>
       </c>
       <c r="F7" t="n">
-        <v>8850211.927541619</v>
+        <v>9241454.34912899</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: Add hybrid model for mortgage prediction and implement data handling
- Introduced `ModeloHipoteca` class for mortgage prediction with data loading, preprocessing, and model training.
- Implemented multicollinearity analysis and validation for input data.
- Added functionality for temporal data preparation and model evaluation with detailed metrics.
- Created visualizations for model predictions and residuals.
- Integrated hybrid model predictions with validation against real data.
- Added JSON and Excel output for predictions and summaries.
- Updated example usage script to reflect new module structure and imports.
- Created new directories and files for organized data storage and example initialization.
</commit_message>
<xml_diff>
--- a/predicciones_produccion.xlsx
+++ b/predicciones_produccion.xlsx
@@ -471,19 +471,19 @@
         <v>45931</v>
       </c>
       <c r="B2" t="n">
-        <v>9241454.34912899</v>
+        <v>9260251.38139425</v>
       </c>
       <c r="C2" t="n">
-        <v>9241454.34912899</v>
+        <v>9260251.38139425</v>
       </c>
       <c r="D2" t="n">
-        <v>9241454.34912899</v>
+        <v>9260251.38139425</v>
       </c>
       <c r="E2" t="n">
-        <v>9241454.34912899</v>
+        <v>9260251.38139425</v>
       </c>
       <c r="F2" t="n">
-        <v>9241454.34912899</v>
+        <v>9260251.38139425</v>
       </c>
     </row>
     <row r="3">
@@ -491,19 +491,19 @@
         <v>45962</v>
       </c>
       <c r="B3" t="n">
-        <v>9241454.34912899</v>
+        <v>9260251.38139425</v>
       </c>
       <c r="C3" t="n">
-        <v>9241454.34912899</v>
+        <v>9260251.38139425</v>
       </c>
       <c r="D3" t="n">
-        <v>9241454.34912899</v>
+        <v>9260251.38139425</v>
       </c>
       <c r="E3" t="n">
-        <v>9241454.34912899</v>
+        <v>9260251.38139425</v>
       </c>
       <c r="F3" t="n">
-        <v>9241454.34912899</v>
+        <v>9260251.38139425</v>
       </c>
     </row>
     <row r="4">
@@ -511,19 +511,19 @@
         <v>45992</v>
       </c>
       <c r="B4" t="n">
-        <v>9241454.34912899</v>
+        <v>9260251.38139425</v>
       </c>
       <c r="C4" t="n">
-        <v>9241454.34912899</v>
+        <v>9260251.38139425</v>
       </c>
       <c r="D4" t="n">
-        <v>9241454.34912899</v>
+        <v>9260251.38139425</v>
       </c>
       <c r="E4" t="n">
-        <v>9241454.34912899</v>
+        <v>9260251.38139425</v>
       </c>
       <c r="F4" t="n">
-        <v>9241454.34912899</v>
+        <v>9260251.38139425</v>
       </c>
     </row>
     <row r="5">
@@ -531,19 +531,19 @@
         <v>46023</v>
       </c>
       <c r="B5" t="n">
-        <v>9241454.34912899</v>
+        <v>9260251.38139425</v>
       </c>
       <c r="C5" t="n">
-        <v>9241454.34912899</v>
+        <v>9260251.38139425</v>
       </c>
       <c r="D5" t="n">
-        <v>9241454.34912899</v>
+        <v>9260251.38139425</v>
       </c>
       <c r="E5" t="n">
-        <v>9241454.34912899</v>
+        <v>9260251.38139425</v>
       </c>
       <c r="F5" t="n">
-        <v>9241454.34912899</v>
+        <v>9260251.38139425</v>
       </c>
     </row>
     <row r="6">
@@ -551,19 +551,19 @@
         <v>46054</v>
       </c>
       <c r="B6" t="n">
-        <v>9241454.34912899</v>
+        <v>9260251.38139425</v>
       </c>
       <c r="C6" t="n">
-        <v>9241454.34912899</v>
+        <v>9260251.38139425</v>
       </c>
       <c r="D6" t="n">
-        <v>9241454.34912899</v>
+        <v>9260251.38139425</v>
       </c>
       <c r="E6" t="n">
-        <v>9241454.34912899</v>
+        <v>9260251.38139425</v>
       </c>
       <c r="F6" t="n">
-        <v>9241454.34912899</v>
+        <v>9260251.38139425</v>
       </c>
     </row>
     <row r="7">
@@ -571,19 +571,19 @@
         <v>46082</v>
       </c>
       <c r="B7" t="n">
-        <v>9241454.34912899</v>
+        <v>9260251.38139425</v>
       </c>
       <c r="C7" t="n">
-        <v>9241454.34912899</v>
+        <v>9260251.38139425</v>
       </c>
       <c r="D7" t="n">
-        <v>9241454.34912899</v>
+        <v>9260251.38139425</v>
       </c>
       <c r="E7" t="n">
-        <v>9241454.34912899</v>
+        <v>9260251.38139425</v>
       </c>
       <c r="F7" t="n">
-        <v>9241454.34912899</v>
+        <v>9260251.38139425</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: Update prediction data handling and enhance data loading capabilities
</commit_message>
<xml_diff>
--- a/predicciones_produccion.xlsx
+++ b/predicciones_produccion.xlsx
@@ -471,19 +471,19 @@
         <v>45931</v>
       </c>
       <c r="B2" t="n">
-        <v>9260251.38139425</v>
+        <v>9255921.002451137</v>
       </c>
       <c r="C2" t="n">
-        <v>9260251.38139425</v>
+        <v>9255921.002451137</v>
       </c>
       <c r="D2" t="n">
-        <v>9260251.38139425</v>
+        <v>9255921.002451137</v>
       </c>
       <c r="E2" t="n">
-        <v>9260251.38139425</v>
+        <v>9255921.002451137</v>
       </c>
       <c r="F2" t="n">
-        <v>9260251.38139425</v>
+        <v>9255921.002451137</v>
       </c>
     </row>
     <row r="3">
@@ -491,19 +491,19 @@
         <v>45962</v>
       </c>
       <c r="B3" t="n">
-        <v>9260251.38139425</v>
+        <v>9255921.002451137</v>
       </c>
       <c r="C3" t="n">
-        <v>9260251.38139425</v>
+        <v>9255921.002451137</v>
       </c>
       <c r="D3" t="n">
-        <v>9260251.38139425</v>
+        <v>9255921.002451137</v>
       </c>
       <c r="E3" t="n">
-        <v>9260251.38139425</v>
+        <v>9255921.002451137</v>
       </c>
       <c r="F3" t="n">
-        <v>9260251.38139425</v>
+        <v>9255921.002451137</v>
       </c>
     </row>
     <row r="4">
@@ -511,19 +511,19 @@
         <v>45992</v>
       </c>
       <c r="B4" t="n">
-        <v>9260251.38139425</v>
+        <v>9255921.002451137</v>
       </c>
       <c r="C4" t="n">
-        <v>9260251.38139425</v>
+        <v>9255921.002451137</v>
       </c>
       <c r="D4" t="n">
-        <v>9260251.38139425</v>
+        <v>9255921.002451137</v>
       </c>
       <c r="E4" t="n">
-        <v>9260251.38139425</v>
+        <v>9255921.002451137</v>
       </c>
       <c r="F4" t="n">
-        <v>9260251.38139425</v>
+        <v>9255921.002451137</v>
       </c>
     </row>
     <row r="5">
@@ -531,19 +531,19 @@
         <v>46023</v>
       </c>
       <c r="B5" t="n">
-        <v>9260251.38139425</v>
+        <v>9255921.002451137</v>
       </c>
       <c r="C5" t="n">
-        <v>9260251.38139425</v>
+        <v>9255921.002451137</v>
       </c>
       <c r="D5" t="n">
-        <v>9260251.38139425</v>
+        <v>9255921.002451137</v>
       </c>
       <c r="E5" t="n">
-        <v>9260251.38139425</v>
+        <v>9255921.002451137</v>
       </c>
       <c r="F5" t="n">
-        <v>9260251.38139425</v>
+        <v>9255921.002451137</v>
       </c>
     </row>
     <row r="6">
@@ -551,19 +551,19 @@
         <v>46054</v>
       </c>
       <c r="B6" t="n">
-        <v>9260251.38139425</v>
+        <v>9255921.002451137</v>
       </c>
       <c r="C6" t="n">
-        <v>9260251.38139425</v>
+        <v>9255921.002451137</v>
       </c>
       <c r="D6" t="n">
-        <v>9260251.38139425</v>
+        <v>9255921.002451137</v>
       </c>
       <c r="E6" t="n">
-        <v>9260251.38139425</v>
+        <v>9255921.002451137</v>
       </c>
       <c r="F6" t="n">
-        <v>9260251.38139425</v>
+        <v>9255921.002451137</v>
       </c>
     </row>
     <row r="7">
@@ -571,19 +571,19 @@
         <v>46082</v>
       </c>
       <c r="B7" t="n">
-        <v>9260251.38139425</v>
+        <v>9255921.002451137</v>
       </c>
       <c r="C7" t="n">
-        <v>9260251.38139425</v>
+        <v>9255921.002451137</v>
       </c>
       <c r="D7" t="n">
-        <v>9260251.38139425</v>
+        <v>9255921.002451137</v>
       </c>
       <c r="E7" t="n">
-        <v>9260251.38139425</v>
+        <v>9255921.002451137</v>
       </c>
       <c r="F7" t="n">
-        <v>9260251.38139425</v>
+        <v>9255921.002451137</v>
       </c>
     </row>
   </sheetData>

</xml_diff>